<commit_message>
Increase file size and self code review
</commit_message>
<xml_diff>
--- a/public/assets/csv/MBC_SAMPLE.xlsx
+++ b/public/assets/csv/MBC_SAMPLE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t xml:space="preserve">ROLE_ID</t>
   </si>
@@ -46,13 +46,13 @@
     <t xml:space="preserve">PARENTS_TO_BE</t>
   </si>
   <si>
-    <t xml:space="preserve">Surrogate1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mother</t>
-  </si>
-  <si>
-    <t xml:space="preserve">surrogate4@yopmail.com</t>
+    <t xml:space="preserve">David</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">david@yopmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">11/3/1988</t>
@@ -61,10 +61,34 @@
     <t xml:space="preserve">SURROGATE_MOTHER</t>
   </si>
   <si>
-    <t xml:space="preserve">Surrogate2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">surrogate8@yopmail.com</t>
+    <t xml:space="preserve">Emma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emma@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGG_DONER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sophia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shophia@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPERM_DONER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James</t>
+  </si>
+  <si>
+    <t xml:space="preserve">william</t>
+  </si>
+  <si>
+    <t xml:space="preserve">james@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -75,7 +99,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -99,6 +123,13 @@
     </font>
     <font>
       <sz val="48"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="48"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -146,7 +177,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -156,6 +187,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -176,10 +211,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="26" zoomScaleNormal="26" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="57.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -255,7 +290,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>9123456789</v>
+        <v>9123477789</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
@@ -264,10 +299,54 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>7777777777</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>8888888888</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" display="shophia@yopmail.com"/>
+    <hyperlink ref="F5" r:id="rId2" display="james@yopmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Chat Media add and get api's
</commit_message>
<xml_diff>
--- a/public/assets/csv/MBC_SAMPLE.xlsx
+++ b/public/assets/csv/MBC_SAMPLE.xlsx
@@ -5,26 +5,26 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KiwiTech\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
-    <sheet name="MBC_REGISTRATION_IMPORT_SAMPLE " sheetId="1" r:id="rId1"/>
+    <sheet name="MBC_REGISTRATION_IMPORT_SAMPLE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>ROLE_ID</t>
   </si>
@@ -50,67 +50,71 @@
     <t>PARENTS_TO_BE</t>
   </si>
   <si>
+    <t>Haden</t>
+  </si>
+  <si>
+    <t>david@yopmail.com</t>
+  </si>
+  <si>
+    <t>SURROGATE_MOTHER</t>
+  </si>
+  <si>
+    <t>emma@yopmail.com</t>
+  </si>
+  <si>
+    <t>EGG_DONER</t>
+  </si>
+  <si>
+    <t>Loren</t>
+  </si>
+  <si>
+    <t>shophia@yopmail.com</t>
+  </si>
+  <si>
+    <t>SPERM_DONER</t>
+  </si>
+  <si>
+    <t>william</t>
+  </si>
+  <si>
+    <t>james@yopmail.com</t>
+  </si>
+  <si>
+    <t>11/6/1988</t>
+  </si>
+  <si>
+    <t>11/7/1988</t>
+  </si>
+  <si>
+    <t>11/8/1988</t>
+  </si>
+  <si>
+    <t>11/9/1988</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Sophia</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
     <t>David</t>
-  </si>
-  <si>
-    <t>Haden</t>
-  </si>
-  <si>
-    <t>david@yopmail.com</t>
-  </si>
-  <si>
-    <t>11/3/1988</t>
-  </si>
-  <si>
-    <t>SURROGATE_MOTHER</t>
-  </si>
-  <si>
-    <t>Emma</t>
-  </si>
-  <si>
-    <t>emma@yopmail.com</t>
-  </si>
-  <si>
-    <t>EGG_DONER</t>
-  </si>
-  <si>
-    <t>Sophia</t>
-  </si>
-  <si>
-    <t>Loren</t>
-  </si>
-  <si>
-    <t>shophia@yopmail.com</t>
-  </si>
-  <si>
-    <t>SPERM_DONER</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>william</t>
-  </si>
-  <si>
-    <t>james@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="48"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,10 +137,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,140 +420,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMA5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="26" zoomScaleNormal="26" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="59.25" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="119.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="58.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="66.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="54.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="51.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="99.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="40.5703125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="178.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="82.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" style="1" customWidth="1"/>
-    <col min="16" max="1015" width="11.5703125" style="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2">
+        <v>9123459789</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1">
-        <v>9123459789</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>9123477789</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1">
-        <v>9123477789</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E4">
+        <v>7777777777</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E5">
+        <v>8888888888</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1">
-        <v>7777777777</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E5" s="1">
-        <v>8888888888</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>